<commit_message>
fixes enumeration issue in environmental metadata xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_environmental_metadata.xlsx
+++ b/data-raw/metadata/camp_environmental_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2CC41F-94B5-3641-842A-2D68E4BB246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FAF14E-2844-6C48-9591-C9A480A343C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-12120" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -526,22 +526,26 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -842,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z958"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21:M21"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -931,7 +935,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1503,7 +1507,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -28029,7 +28033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z931"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A93" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
creates visitType column for environmental table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_environmental_metadata.xlsx
+++ b/data-raw/metadata/camp_environmental_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B337CF0-EAF9-4240-9D74-720F366ED451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70206C4-F2C5-F042-9C70-E0D317B9CEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -157,12 +157,6 @@
     <t>Date and time of day associated with the trap visit. Definition varies based on visitType (For visitTypeID=1, 2, or 3 this is the date and the time of day the trap began fishing. For visitTypeID=4, 5, or 6 this is the date and the time of day of the end of the visit.)</t>
   </si>
   <si>
-    <t>visitTypeID</t>
-  </si>
-  <si>
-    <t>Code for work that was done during visit to trap</t>
-  </si>
-  <si>
     <t>siteID</t>
   </si>
   <si>
@@ -245,33 +239,6 @@
   </si>
   <si>
     <t>Unknown</t>
-  </si>
-  <si>
-    <t>Not applicable (n/a)</t>
-  </si>
-  <si>
-    <t>Continue trapping</t>
-  </si>
-  <si>
-    <t>Drive-by only</t>
-  </si>
-  <si>
-    <t>End trapping</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>See Comments</t>
-  </si>
-  <si>
-    <t>Service/adjust/clean trap</t>
-  </si>
-  <si>
-    <t>Start trap &amp; begin trapping</t>
-  </si>
-  <si>
-    <t>Unplanned restart</t>
   </si>
   <si>
     <t>see unit column</t>
@@ -360,6 +327,14 @@
   </si>
   <si>
     <t>Code for position of trap within the site. Levels = c(63004, 63003)</t>
+  </si>
+  <si>
+    <t>Work that was done during visit to trap. Levels = c("Continue trapping", "End trapping", "Start trap &amp; begin trapping", 
+"Unplanned restart", "Service/adjust/clean trap", "Drive-by only"
+)</t>
+  </si>
+  <si>
+    <t>visitType</t>
   </si>
 </sst>
 </file>
@@ -695,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z948"/>
+  <dimension ref="A1:Z947"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -906,7 +881,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>28</v>
@@ -954,7 +929,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>28</v>
@@ -1002,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>28</v>
@@ -1050,7 +1025,7 @@
         <v>26</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>28</v>
@@ -1098,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>28</v>
@@ -1151,10 +1126,10 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="17" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1195,10 +1170,10 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="17" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1234,9 +1209,9 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="3"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1254,10 +1229,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1266,7 +1241,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1292,10 +1267,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1310,9 +1285,9 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1330,10 +1305,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1368,10 +1343,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
@@ -1406,10 +1381,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -1444,10 +1419,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1482,10 +1457,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1520,10 +1495,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -1558,10 +1533,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -1596,10 +1571,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
@@ -1634,10 +1609,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
@@ -1671,16 +1646,16 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>95</v>
+      <c r="A24" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -27552,46 +27527,18 @@
       <c r="Y947" s="1"/>
       <c r="Z947" s="1"/>
     </row>
-    <row r="948" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A948" s="1"/>
-      <c r="B948" s="1"/>
-      <c r="C948" s="1"/>
-      <c r="D948" s="2"/>
-      <c r="E948" s="1"/>
-      <c r="F948" s="3"/>
-      <c r="G948" s="3"/>
-      <c r="H948" s="3"/>
-      <c r="I948" s="2"/>
-      <c r="J948" s="3"/>
-      <c r="K948" s="2"/>
-      <c r="L948" s="3"/>
-      <c r="M948" s="3"/>
-      <c r="N948" s="1"/>
-      <c r="O948" s="1"/>
-      <c r="P948" s="1"/>
-      <c r="Q948" s="1"/>
-      <c r="R948" s="1"/>
-      <c r="S948" s="1"/>
-      <c r="T948" s="1"/>
-      <c r="U948" s="1"/>
-      <c r="V948" s="1"/>
-      <c r="W948" s="1"/>
-      <c r="X948" s="1"/>
-      <c r="Y948" s="1"/>
-      <c r="Z948" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E15 E16:E948" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E947" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F15 F16:F948" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F947" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C15 C16:C948" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C947" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H15 H16:H948" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H947" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27602,10 +27549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z842"/>
+  <dimension ref="A1:Z830"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="A26" sqref="A26:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27618,13 +27565,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -27655,7 +27602,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -27689,10 +27636,10 @@
         <v>3000</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -27723,10 +27670,10 @@
         <v>44000</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -27757,10 +27704,10 @@
         <v>52000</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -27791,10 +27738,10 @@
         <v>51000</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -27825,10 +27772,10 @@
         <v>5000</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -27859,10 +27806,10 @@
         <v>46000</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -27893,10 +27840,10 @@
         <v>4000</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -27927,10 +27874,10 @@
         <v>45000</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -27961,10 +27908,10 @@
         <v>252</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -27995,10 +27942,10 @@
         <v>251</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -28029,10 +27976,10 @@
         <v>255</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -28063,10 +28010,10 @@
         <v>53000</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -28097,10 +28044,10 @@
         <v>54000</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -28131,10 +28078,10 @@
         <v>55000</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -28165,10 +28112,10 @@
         <v>56000</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -28199,10 +28146,10 @@
         <v>50000</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -28233,10 +28180,10 @@
         <v>7000</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -28267,10 +28214,10 @@
         <v>2000</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -28301,10 +28248,10 @@
         <v>43000</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -28335,10 +28282,10 @@
         <v>6000</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -28369,10 +28316,10 @@
         <v>47000</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -28403,10 +28350,10 @@
         <v>90000</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -28437,10 +28384,10 @@
         <v>253</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -28467,15 +28414,9 @@
       <c r="Z25" s="16"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
-        <v>2</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -28501,15 +28442,9 @@
       <c r="Z26" s="16"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
-        <v>5</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -28535,15 +28470,9 @@
       <c r="Z27" s="16"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
-        <v>4</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -28569,15 +28498,9 @@
       <c r="Z28" s="16"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
-        <v>252</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -28603,15 +28526,9 @@
       <c r="Z29" s="16"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
-        <v>251</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -28637,15 +28554,9 @@
       <c r="Z30" s="16"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
-        <v>255</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
@@ -28671,15 +28582,9 @@
       <c r="Z31" s="16"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
-        <v>250</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
@@ -28705,15 +28610,9 @@
       <c r="Z32" s="16"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
-        <v>254</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
@@ -28739,15 +28638,9 @@
       <c r="Z33" s="16"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
-        <v>6</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -28773,15 +28666,9 @@
       <c r="Z34" s="16"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
-        <v>1</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -28807,15 +28694,9 @@
       <c r="Z35" s="16"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16">
-        <v>253</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
@@ -28841,15 +28722,9 @@
       <c r="Z36" s="16"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
-        <v>3</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -51078,342 +50953,6 @@
       <c r="Y830" s="16"/>
       <c r="Z830" s="16"/>
     </row>
-    <row r="831" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A831" s="15"/>
-      <c r="B831" s="15"/>
-      <c r="C831" s="15"/>
-      <c r="D831" s="16"/>
-      <c r="E831" s="16"/>
-      <c r="F831" s="16"/>
-      <c r="G831" s="16"/>
-      <c r="H831" s="16"/>
-      <c r="I831" s="16"/>
-      <c r="J831" s="16"/>
-      <c r="K831" s="16"/>
-      <c r="L831" s="16"/>
-      <c r="M831" s="16"/>
-      <c r="N831" s="16"/>
-      <c r="O831" s="16"/>
-      <c r="P831" s="16"/>
-      <c r="Q831" s="16"/>
-      <c r="R831" s="16"/>
-      <c r="S831" s="16"/>
-      <c r="T831" s="16"/>
-      <c r="U831" s="16"/>
-      <c r="V831" s="16"/>
-      <c r="W831" s="16"/>
-      <c r="X831" s="16"/>
-      <c r="Y831" s="16"/>
-      <c r="Z831" s="16"/>
-    </row>
-    <row r="832" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A832" s="15"/>
-      <c r="B832" s="15"/>
-      <c r="C832" s="15"/>
-      <c r="D832" s="16"/>
-      <c r="E832" s="16"/>
-      <c r="F832" s="16"/>
-      <c r="G832" s="16"/>
-      <c r="H832" s="16"/>
-      <c r="I832" s="16"/>
-      <c r="J832" s="16"/>
-      <c r="K832" s="16"/>
-      <c r="L832" s="16"/>
-      <c r="M832" s="16"/>
-      <c r="N832" s="16"/>
-      <c r="O832" s="16"/>
-      <c r="P832" s="16"/>
-      <c r="Q832" s="16"/>
-      <c r="R832" s="16"/>
-      <c r="S832" s="16"/>
-      <c r="T832" s="16"/>
-      <c r="U832" s="16"/>
-      <c r="V832" s="16"/>
-      <c r="W832" s="16"/>
-      <c r="X832" s="16"/>
-      <c r="Y832" s="16"/>
-      <c r="Z832" s="16"/>
-    </row>
-    <row r="833" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A833" s="15"/>
-      <c r="B833" s="15"/>
-      <c r="C833" s="15"/>
-      <c r="D833" s="16"/>
-      <c r="E833" s="16"/>
-      <c r="F833" s="16"/>
-      <c r="G833" s="16"/>
-      <c r="H833" s="16"/>
-      <c r="I833" s="16"/>
-      <c r="J833" s="16"/>
-      <c r="K833" s="16"/>
-      <c r="L833" s="16"/>
-      <c r="M833" s="16"/>
-      <c r="N833" s="16"/>
-      <c r="O833" s="16"/>
-      <c r="P833" s="16"/>
-      <c r="Q833" s="16"/>
-      <c r="R833" s="16"/>
-      <c r="S833" s="16"/>
-      <c r="T833" s="16"/>
-      <c r="U833" s="16"/>
-      <c r="V833" s="16"/>
-      <c r="W833" s="16"/>
-      <c r="X833" s="16"/>
-      <c r="Y833" s="16"/>
-      <c r="Z833" s="16"/>
-    </row>
-    <row r="834" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A834" s="15"/>
-      <c r="B834" s="15"/>
-      <c r="C834" s="15"/>
-      <c r="D834" s="16"/>
-      <c r="E834" s="16"/>
-      <c r="F834" s="16"/>
-      <c r="G834" s="16"/>
-      <c r="H834" s="16"/>
-      <c r="I834" s="16"/>
-      <c r="J834" s="16"/>
-      <c r="K834" s="16"/>
-      <c r="L834" s="16"/>
-      <c r="M834" s="16"/>
-      <c r="N834" s="16"/>
-      <c r="O834" s="16"/>
-      <c r="P834" s="16"/>
-      <c r="Q834" s="16"/>
-      <c r="R834" s="16"/>
-      <c r="S834" s="16"/>
-      <c r="T834" s="16"/>
-      <c r="U834" s="16"/>
-      <c r="V834" s="16"/>
-      <c r="W834" s="16"/>
-      <c r="X834" s="16"/>
-      <c r="Y834" s="16"/>
-      <c r="Z834" s="16"/>
-    </row>
-    <row r="835" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A835" s="15"/>
-      <c r="B835" s="15"/>
-      <c r="C835" s="15"/>
-      <c r="D835" s="16"/>
-      <c r="E835" s="16"/>
-      <c r="F835" s="16"/>
-      <c r="G835" s="16"/>
-      <c r="H835" s="16"/>
-      <c r="I835" s="16"/>
-      <c r="J835" s="16"/>
-      <c r="K835" s="16"/>
-      <c r="L835" s="16"/>
-      <c r="M835" s="16"/>
-      <c r="N835" s="16"/>
-      <c r="O835" s="16"/>
-      <c r="P835" s="16"/>
-      <c r="Q835" s="16"/>
-      <c r="R835" s="16"/>
-      <c r="S835" s="16"/>
-      <c r="T835" s="16"/>
-      <c r="U835" s="16"/>
-      <c r="V835" s="16"/>
-      <c r="W835" s="16"/>
-      <c r="X835" s="16"/>
-      <c r="Y835" s="16"/>
-      <c r="Z835" s="16"/>
-    </row>
-    <row r="836" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A836" s="15"/>
-      <c r="B836" s="15"/>
-      <c r="C836" s="15"/>
-      <c r="D836" s="16"/>
-      <c r="E836" s="16"/>
-      <c r="F836" s="16"/>
-      <c r="G836" s="16"/>
-      <c r="H836" s="16"/>
-      <c r="I836" s="16"/>
-      <c r="J836" s="16"/>
-      <c r="K836" s="16"/>
-      <c r="L836" s="16"/>
-      <c r="M836" s="16"/>
-      <c r="N836" s="16"/>
-      <c r="O836" s="16"/>
-      <c r="P836" s="16"/>
-      <c r="Q836" s="16"/>
-      <c r="R836" s="16"/>
-      <c r="S836" s="16"/>
-      <c r="T836" s="16"/>
-      <c r="U836" s="16"/>
-      <c r="V836" s="16"/>
-      <c r="W836" s="16"/>
-      <c r="X836" s="16"/>
-      <c r="Y836" s="16"/>
-      <c r="Z836" s="16"/>
-    </row>
-    <row r="837" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A837" s="15"/>
-      <c r="B837" s="15"/>
-      <c r="C837" s="15"/>
-      <c r="D837" s="16"/>
-      <c r="E837" s="16"/>
-      <c r="F837" s="16"/>
-      <c r="G837" s="16"/>
-      <c r="H837" s="16"/>
-      <c r="I837" s="16"/>
-      <c r="J837" s="16"/>
-      <c r="K837" s="16"/>
-      <c r="L837" s="16"/>
-      <c r="M837" s="16"/>
-      <c r="N837" s="16"/>
-      <c r="O837" s="16"/>
-      <c r="P837" s="16"/>
-      <c r="Q837" s="16"/>
-      <c r="R837" s="16"/>
-      <c r="S837" s="16"/>
-      <c r="T837" s="16"/>
-      <c r="U837" s="16"/>
-      <c r="V837" s="16"/>
-      <c r="W837" s="16"/>
-      <c r="X837" s="16"/>
-      <c r="Y837" s="16"/>
-      <c r="Z837" s="16"/>
-    </row>
-    <row r="838" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A838" s="15"/>
-      <c r="B838" s="15"/>
-      <c r="C838" s="15"/>
-      <c r="D838" s="16"/>
-      <c r="E838" s="16"/>
-      <c r="F838" s="16"/>
-      <c r="G838" s="16"/>
-      <c r="H838" s="16"/>
-      <c r="I838" s="16"/>
-      <c r="J838" s="16"/>
-      <c r="K838" s="16"/>
-      <c r="L838" s="16"/>
-      <c r="M838" s="16"/>
-      <c r="N838" s="16"/>
-      <c r="O838" s="16"/>
-      <c r="P838" s="16"/>
-      <c r="Q838" s="16"/>
-      <c r="R838" s="16"/>
-      <c r="S838" s="16"/>
-      <c r="T838" s="16"/>
-      <c r="U838" s="16"/>
-      <c r="V838" s="16"/>
-      <c r="W838" s="16"/>
-      <c r="X838" s="16"/>
-      <c r="Y838" s="16"/>
-      <c r="Z838" s="16"/>
-    </row>
-    <row r="839" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A839" s="15"/>
-      <c r="B839" s="15"/>
-      <c r="C839" s="15"/>
-      <c r="D839" s="16"/>
-      <c r="E839" s="16"/>
-      <c r="F839" s="16"/>
-      <c r="G839" s="16"/>
-      <c r="H839" s="16"/>
-      <c r="I839" s="16"/>
-      <c r="J839" s="16"/>
-      <c r="K839" s="16"/>
-      <c r="L839" s="16"/>
-      <c r="M839" s="16"/>
-      <c r="N839" s="16"/>
-      <c r="O839" s="16"/>
-      <c r="P839" s="16"/>
-      <c r="Q839" s="16"/>
-      <c r="R839" s="16"/>
-      <c r="S839" s="16"/>
-      <c r="T839" s="16"/>
-      <c r="U839" s="16"/>
-      <c r="V839" s="16"/>
-      <c r="W839" s="16"/>
-      <c r="X839" s="16"/>
-      <c r="Y839" s="16"/>
-      <c r="Z839" s="16"/>
-    </row>
-    <row r="840" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A840" s="15"/>
-      <c r="B840" s="15"/>
-      <c r="C840" s="15"/>
-      <c r="D840" s="16"/>
-      <c r="E840" s="16"/>
-      <c r="F840" s="16"/>
-      <c r="G840" s="16"/>
-      <c r="H840" s="16"/>
-      <c r="I840" s="16"/>
-      <c r="J840" s="16"/>
-      <c r="K840" s="16"/>
-      <c r="L840" s="16"/>
-      <c r="M840" s="16"/>
-      <c r="N840" s="16"/>
-      <c r="O840" s="16"/>
-      <c r="P840" s="16"/>
-      <c r="Q840" s="16"/>
-      <c r="R840" s="16"/>
-      <c r="S840" s="16"/>
-      <c r="T840" s="16"/>
-      <c r="U840" s="16"/>
-      <c r="V840" s="16"/>
-      <c r="W840" s="16"/>
-      <c r="X840" s="16"/>
-      <c r="Y840" s="16"/>
-      <c r="Z840" s="16"/>
-    </row>
-    <row r="841" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A841" s="15"/>
-      <c r="B841" s="15"/>
-      <c r="C841" s="15"/>
-      <c r="D841" s="16"/>
-      <c r="E841" s="16"/>
-      <c r="F841" s="16"/>
-      <c r="G841" s="16"/>
-      <c r="H841" s="16"/>
-      <c r="I841" s="16"/>
-      <c r="J841" s="16"/>
-      <c r="K841" s="16"/>
-      <c r="L841" s="16"/>
-      <c r="M841" s="16"/>
-      <c r="N841" s="16"/>
-      <c r="O841" s="16"/>
-      <c r="P841" s="16"/>
-      <c r="Q841" s="16"/>
-      <c r="R841" s="16"/>
-      <c r="S841" s="16"/>
-      <c r="T841" s="16"/>
-      <c r="U841" s="16"/>
-      <c r="V841" s="16"/>
-      <c r="W841" s="16"/>
-      <c r="X841" s="16"/>
-      <c r="Y841" s="16"/>
-      <c r="Z841" s="16"/>
-    </row>
-    <row r="842" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A842" s="15"/>
-      <c r="B842" s="15"/>
-      <c r="C842" s="15"/>
-      <c r="D842" s="16"/>
-      <c r="E842" s="16"/>
-      <c r="F842" s="16"/>
-      <c r="G842" s="16"/>
-      <c r="H842" s="16"/>
-      <c r="I842" s="16"/>
-      <c r="J842" s="16"/>
-      <c r="K842" s="16"/>
-      <c r="L842" s="16"/>
-      <c r="M842" s="16"/>
-      <c r="N842" s="16"/>
-      <c r="O842" s="16"/>
-      <c r="P842" s="16"/>
-      <c r="Q842" s="16"/>
-      <c r="R842" s="16"/>
-      <c r="S842" s="16"/>
-      <c r="T842" s="16"/>
-      <c r="U842" s="16"/>
-      <c r="V842" s="16"/>
-      <c r="W842" s="16"/>
-      <c r="X842" s="16"/>
-      <c r="Y842" s="16"/>
-      <c r="Z842" s="16"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
removes unit columns. adds units from methods to metadata attributes. validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_environmental_metadata.xlsx
+++ b/data-raw/metadata/camp_environmental_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70206C4-F2C5-F042-9C70-E0D317B9CEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38CB2BA-CF68-7C45-8089-AB5FA9129DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -241,9 +241,6 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>see unit column</t>
-  </si>
-  <si>
     <t>2006-10-02 02:30:00</t>
   </si>
   <si>
@@ -253,57 +250,23 @@
     <t>Knights Landing RST Program</t>
   </si>
   <si>
-    <t>dischargeUnit</t>
-  </si>
-  <si>
     <t>dischargeSampleGear</t>
-  </si>
-  <si>
-    <t>waterVelUnit</t>
   </si>
   <si>
     <t>waterVelSampleGear</t>
   </si>
   <si>
-    <t>waterTempUnit</t>
-  </si>
-  <si>
     <t>waterTempSampleGear</t>
-  </si>
-  <si>
-    <t>lightPenetrationUnit</t>
   </si>
   <si>
     <t>lightPenetrationSampleGear</t>
   </si>
   <si>
-    <t>turbidityUnit</t>
-  </si>
-  <si>
     <t>turbiditySampleGear</t>
-  </si>
-  <si>
-    <t>Unit of measure. Levels = c("cubic feet/second (cfs)", NA, "Not recorded", "centimeter (cm)", 
-"nephelometric turbidity units (NTU)", "feet/second (ft/sec)", 
-"cubic meters/second (m3/sec)")</t>
   </si>
   <si>
     <t>The sample gear used. Levels = c("Gauging station (non-USGS)", NA, "Electronic meter", "Electronic depth finder", 
 "Not recorded")</t>
-  </si>
-  <si>
-    <t>Unit of measure. Levels = c("feet/second (ft/sec)", NA, "Not recorded", "cubic feet/second (cfs)", 
-"meters/second (m/sec)", "meter (m)")</t>
-  </si>
-  <si>
-    <t>Unit of measure. Levels = c(NA, "Not recorded", "feet/second (ft/sec)", "C")</t>
-  </si>
-  <si>
-    <t>Unit of measure. Levels = c(NA, "Not recorded", "percent (%)", "centimeter (cm)")</t>
-  </si>
-  <si>
-    <t>Unit of measure. Levels = c("nephelometric turbidity units (NTU)", NA, "Not recorded", 
-"meters/second (m/sec)")</t>
   </si>
   <si>
     <t>The sample gear used. Levels = c("Electronic meter", NA, "Not recorded", "Electronic depth finder"
@@ -335,6 +298,21 @@
   </si>
   <si>
     <t>visitType</t>
+  </si>
+  <si>
+    <t>cubicFeetPerSecond</t>
+  </si>
+  <si>
+    <t>metersPerSecond</t>
+  </si>
+  <si>
+    <t>celsius</t>
+  </si>
+  <si>
+    <t>Nephelometric Turbidity Units (NTU)</t>
+  </si>
+  <si>
+    <t>centimeter</t>
   </si>
 </sst>
 </file>
@@ -670,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z947"/>
+  <dimension ref="A1:Z942"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -881,7 +859,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>28</v>
@@ -929,7 +907,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>28</v>
@@ -977,7 +955,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>28</v>
@@ -1025,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>28</v>
@@ -1073,7 +1051,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>28</v>
@@ -1126,10 +1104,10 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1170,10 +1148,10 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1229,10 +1207,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1267,10 +1245,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1305,10 +1283,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1343,10 +1321,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
@@ -1381,10 +1359,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -1419,10 +1397,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1456,8 +1434,8 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>76</v>
+      <c r="A19" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
@@ -1465,7 +1443,7 @@
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1494,21 +1472,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1532,21 +1500,11 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1570,21 +1528,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1608,21 +1556,11 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1646,21 +1584,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -27387,158 +27315,18 @@
       <c r="Y942" s="1"/>
       <c r="Z942" s="1"/>
     </row>
-    <row r="943" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A943" s="1"/>
-      <c r="B943" s="1"/>
-      <c r="C943" s="1"/>
-      <c r="D943" s="2"/>
-      <c r="E943" s="1"/>
-      <c r="F943" s="3"/>
-      <c r="G943" s="3"/>
-      <c r="H943" s="3"/>
-      <c r="I943" s="2"/>
-      <c r="J943" s="3"/>
-      <c r="K943" s="2"/>
-      <c r="L943" s="3"/>
-      <c r="M943" s="3"/>
-      <c r="N943" s="1"/>
-      <c r="O943" s="1"/>
-      <c r="P943" s="1"/>
-      <c r="Q943" s="1"/>
-      <c r="R943" s="1"/>
-      <c r="S943" s="1"/>
-      <c r="T943" s="1"/>
-      <c r="U943" s="1"/>
-      <c r="V943" s="1"/>
-      <c r="W943" s="1"/>
-      <c r="X943" s="1"/>
-      <c r="Y943" s="1"/>
-      <c r="Z943" s="1"/>
-    </row>
-    <row r="944" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A944" s="1"/>
-      <c r="B944" s="1"/>
-      <c r="C944" s="1"/>
-      <c r="D944" s="2"/>
-      <c r="E944" s="1"/>
-      <c r="F944" s="3"/>
-      <c r="G944" s="3"/>
-      <c r="H944" s="3"/>
-      <c r="I944" s="2"/>
-      <c r="J944" s="3"/>
-      <c r="K944" s="2"/>
-      <c r="L944" s="3"/>
-      <c r="M944" s="3"/>
-      <c r="N944" s="1"/>
-      <c r="O944" s="1"/>
-      <c r="P944" s="1"/>
-      <c r="Q944" s="1"/>
-      <c r="R944" s="1"/>
-      <c r="S944" s="1"/>
-      <c r="T944" s="1"/>
-      <c r="U944" s="1"/>
-      <c r="V944" s="1"/>
-      <c r="W944" s="1"/>
-      <c r="X944" s="1"/>
-      <c r="Y944" s="1"/>
-      <c r="Z944" s="1"/>
-    </row>
-    <row r="945" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A945" s="1"/>
-      <c r="B945" s="1"/>
-      <c r="C945" s="1"/>
-      <c r="D945" s="2"/>
-      <c r="E945" s="1"/>
-      <c r="F945" s="3"/>
-      <c r="G945" s="3"/>
-      <c r="H945" s="3"/>
-      <c r="I945" s="2"/>
-      <c r="J945" s="3"/>
-      <c r="K945" s="2"/>
-      <c r="L945" s="3"/>
-      <c r="M945" s="3"/>
-      <c r="N945" s="1"/>
-      <c r="O945" s="1"/>
-      <c r="P945" s="1"/>
-      <c r="Q945" s="1"/>
-      <c r="R945" s="1"/>
-      <c r="S945" s="1"/>
-      <c r="T945" s="1"/>
-      <c r="U945" s="1"/>
-      <c r="V945" s="1"/>
-      <c r="W945" s="1"/>
-      <c r="X945" s="1"/>
-      <c r="Y945" s="1"/>
-      <c r="Z945" s="1"/>
-    </row>
-    <row r="946" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A946" s="1"/>
-      <c r="B946" s="1"/>
-      <c r="C946" s="1"/>
-      <c r="D946" s="2"/>
-      <c r="E946" s="1"/>
-      <c r="F946" s="3"/>
-      <c r="G946" s="3"/>
-      <c r="H946" s="3"/>
-      <c r="I946" s="2"/>
-      <c r="J946" s="3"/>
-      <c r="K946" s="2"/>
-      <c r="L946" s="3"/>
-      <c r="M946" s="3"/>
-      <c r="N946" s="1"/>
-      <c r="O946" s="1"/>
-      <c r="P946" s="1"/>
-      <c r="Q946" s="1"/>
-      <c r="R946" s="1"/>
-      <c r="S946" s="1"/>
-      <c r="T946" s="1"/>
-      <c r="U946" s="1"/>
-      <c r="V946" s="1"/>
-      <c r="W946" s="1"/>
-      <c r="X946" s="1"/>
-      <c r="Y946" s="1"/>
-      <c r="Z946" s="1"/>
-    </row>
-    <row r="947" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A947" s="1"/>
-      <c r="B947" s="1"/>
-      <c r="C947" s="1"/>
-      <c r="D947" s="2"/>
-      <c r="E947" s="1"/>
-      <c r="F947" s="3"/>
-      <c r="G947" s="3"/>
-      <c r="H947" s="3"/>
-      <c r="I947" s="2"/>
-      <c r="J947" s="3"/>
-      <c r="K947" s="2"/>
-      <c r="L947" s="3"/>
-      <c r="M947" s="3"/>
-      <c r="N947" s="1"/>
-      <c r="O947" s="1"/>
-      <c r="P947" s="1"/>
-      <c r="Q947" s="1"/>
-      <c r="R947" s="1"/>
-      <c r="S947" s="1"/>
-      <c r="T947" s="1"/>
-      <c r="U947" s="1"/>
-      <c r="V947" s="1"/>
-      <c r="W947" s="1"/>
-      <c r="X947" s="1"/>
-      <c r="Y947" s="1"/>
-      <c r="Z947" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E947" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E942" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F947" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F942" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C947" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C942" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H947" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H942" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27602,7 +27390,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>

</xml_diff>